<commit_message>
Update 2 added comments excel function Activity 6
</commit_message>
<xml_diff>
--- a/BookIn_WFANet1/dataXls/TEMPLATE/BookReport.xlsx
+++ b/BookIn_WFANet1/dataXls/TEMPLATE/BookReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\EDP_BookIn\BookIn_WFANet1\dataXls\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCB55B7-6D38-42BF-9B98-9A62823F32E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DD6F58-AA17-4C6A-9F85-F647D407F77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,17 +48,17 @@
     <t>Publisher ID</t>
   </si>
   <si>
-    <t>CUSTOMER REPORT</t>
-  </si>
-  <si>
     <t>Version 1</t>
+  </si>
+  <si>
+    <t>BOOK REPORT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +70,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -119,12 +127,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,7 +555,7 @@
   <dimension ref="A2:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,18 +571,18 @@
       <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
+      <c r="A5" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G6" s="5" t="s">
-        <v>8</v>
+      <c r="G6" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -604,6 +613,7 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>